<commit_message>
3D - Stat UI
</commit_message>
<xml_diff>
--- a/3D/1ST/ArenaBattle/GameData/ABCharacterStatTable.xlsx
+++ b/3D/1ST/ArenaBattle/GameData/ABCharacterStatTable.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2024학년도\1.수업관련\3D 게임프로그래밍\1학기 수업\Asset\GameData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\GitHub\2024_GGM_Study\3D\1ST\ArenaBattle\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B818D4-E27B-4AD8-9EA6-ABDBE6874434}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976" xr2:uid="{14535CBB-5647-4022-885E-3A0FC95BEC4B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12165"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -84,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,21 +443,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D538BA-27C2-42AB-99FE-D911400E397E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C2" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="1"/>
-    <col min="4" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.75" style="1"/>
+    <col min="4" max="5" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -478,7 +477,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -486,7 +485,7 @@
         <v>100</v>
       </c>
       <c r="C2" s="1">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="D2" s="1">
         <v>40</v>
@@ -498,7 +497,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -506,7 +505,7 @@
         <v>150</v>
       </c>
       <c r="C3" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1">
         <v>40</v>
@@ -518,7 +517,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -526,7 +525,7 @@
         <v>200</v>
       </c>
       <c r="C4" s="1">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D4" s="1">
         <v>40</v>
@@ -538,7 +537,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -558,7 +557,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -566,7 +565,7 @@
         <v>300</v>
       </c>
       <c r="C6" s="1">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D6" s="1">
         <v>40</v>
@@ -578,7 +577,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -586,7 +585,7 @@
         <v>350</v>
       </c>
       <c r="C7" s="1">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="D7" s="1">
         <v>40</v>
@@ -598,7 +597,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -606,7 +605,7 @@
         <v>400</v>
       </c>
       <c r="C8" s="1">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D8" s="1">
         <v>40</v>
@@ -618,7 +617,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -626,7 +625,7 @@
         <v>450</v>
       </c>
       <c r="C9" s="1">
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="D9" s="1">
         <v>40</v>
@@ -638,7 +637,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -646,7 +645,7 @@
         <v>500</v>
       </c>
       <c r="C10" s="1">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="D10" s="1">
         <v>40</v>
@@ -658,7 +657,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -666,7 +665,7 @@
         <v>550</v>
       </c>
       <c r="C11" s="1">
-        <v>280</v>
+        <v>400</v>
       </c>
       <c r="D11" s="1">
         <v>40</v>
@@ -681,5 +680,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3D - DownLoad Project
</commit_message>
<xml_diff>
--- a/3D/1ST/ArenaBattle/GameData/ABCharacterStatTable.xlsx
+++ b/3D/1ST/ArenaBattle/GameData/ABCharacterStatTable.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\GitHub\2024_GGM_Study\3D\1ST\ArenaBattle\GameData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2024학년도\1.수업관련\3D 게임프로그래밍\1학기 수업\Asset\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B818D4-E27B-4AD8-9EA6-ABDBE6874434}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976" xr2:uid="{14535CBB-5647-4022-885E-3A0FC95BEC4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -443,21 +444,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3D538BA-27C2-42AB-99FE-D911400E397E}">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="8.75" style="1"/>
-    <col min="4" max="5" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="1"/>
+    <col min="4" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -477,7 +478,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -485,7 +486,7 @@
         <v>100</v>
       </c>
       <c r="C2" s="1">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D2" s="1">
         <v>40</v>
@@ -497,7 +498,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -505,7 +506,7 @@
         <v>150</v>
       </c>
       <c r="C3" s="1">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="D3" s="1">
         <v>40</v>
@@ -517,7 +518,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -525,7 +526,7 @@
         <v>200</v>
       </c>
       <c r="C4" s="1">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D4" s="1">
         <v>40</v>
@@ -537,7 +538,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -557,7 +558,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -565,7 +566,7 @@
         <v>300</v>
       </c>
       <c r="C6" s="1">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="D6" s="1">
         <v>40</v>
@@ -577,7 +578,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -585,7 +586,7 @@
         <v>350</v>
       </c>
       <c r="C7" s="1">
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="D7" s="1">
         <v>40</v>
@@ -597,7 +598,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -605,7 +606,7 @@
         <v>400</v>
       </c>
       <c r="C8" s="1">
-        <v>280</v>
+        <v>220</v>
       </c>
       <c r="D8" s="1">
         <v>40</v>
@@ -617,7 +618,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -625,7 +626,7 @@
         <v>450</v>
       </c>
       <c r="C9" s="1">
-        <v>320</v>
+        <v>240</v>
       </c>
       <c r="D9" s="1">
         <v>40</v>
@@ -637,7 +638,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -645,7 +646,7 @@
         <v>500</v>
       </c>
       <c r="C10" s="1">
-        <v>360</v>
+        <v>260</v>
       </c>
       <c r="D10" s="1">
         <v>40</v>
@@ -657,7 +658,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -665,7 +666,7 @@
         <v>550</v>
       </c>
       <c r="C11" s="1">
-        <v>400</v>
+        <v>280</v>
       </c>
       <c r="D11" s="1">
         <v>40</v>
@@ -680,6 +681,5 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>